<commit_message>
Change columns language in table and script
</commit_message>
<xml_diff>
--- a/wine.xlsx
+++ b/wine.xlsx
@@ -22,22 +22,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sort</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Picture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discount</t>
+    <t xml:space="preserve">Категория</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Имя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сорт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Цена</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Картинка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Акция</t>
   </si>
   <si>
     <t xml:space="preserve">Белые вина</t>
@@ -254,15 +254,15 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.44"/>

</xml_diff>